<commit_message>
Refactor Excel data handling across components: Update DashboardPage to load all Excel files on mount, enforce Excel mode in customer, invoice, and product forms, and streamline product API interactions to utilize Excel API endpoints for fetching, creating, updating, and deleting products. This enhances data consistency and user experience.
</commit_message>
<xml_diff>
--- a/tmp/Products.xlsx
+++ b/tmp/Products.xlsx
@@ -1,41 +1,89 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\billing-solutions\tmp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F517EE95-741F-4E7C-B531-A1BA5016C667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>sku</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>cost_price</t>
+  </si>
+  <si>
+    <t>stock_quantity</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>hsn_code</t>
+  </si>
+  <si>
+    <t>gst_rate</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Sample Product</t>
+  </si>
+  <si>
+    <t>SP-001</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>piece</t>
+  </si>
+  <si>
+    <t>9000</t>
+  </si>
+  <si>
+    <t>Hassan</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -65,13 +113,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,59 +452,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>id</v>
-      </c>
-      <c r="B1" t="str">
-        <v>name</v>
-      </c>
-      <c r="C1" t="str">
-        <v>sku</v>
-      </c>
-      <c r="D1" t="str">
-        <v>category</v>
-      </c>
-      <c r="E1" t="str">
-        <v>price</v>
-      </c>
-      <c r="F1" t="str">
-        <v>cost_price</v>
-      </c>
-      <c r="G1" t="str">
-        <v>stock_quantity</v>
-      </c>
-      <c r="H1" t="str">
-        <v>unit</v>
-      </c>
-      <c r="I1" t="str">
-        <v>hsn_code</v>
-      </c>
-      <c r="J1" t="str">
-        <v>gst_rate</v>
-      </c>
-      <c r="K1" t="str">
-        <v>is_active</v>
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>1</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Sample Product</v>
-      </c>
-      <c r="C2" t="str">
-        <v>SP-001</v>
-      </c>
-      <c r="D2" t="str">
-        <v>QA</v>
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
       </c>
       <c r="E2">
         <v>100</v>
@@ -459,11 +518,11 @@
       <c r="G2">
         <v>10</v>
       </c>
-      <c r="H2" t="str">
-        <v>piece</v>
-      </c>
-      <c r="I2" t="str">
-        <v>9000</v>
+      <c r="H2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
       </c>
       <c r="J2">
         <v>18</v>
@@ -472,9 +531,45 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>200</v>
+      </c>
+      <c r="F3">
+        <v>30</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3">
+        <v>300</v>
+      </c>
+      <c r="J3">
+        <v>18</v>
+      </c>
+      <c r="K3" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:K2"/>
+    <ignoredError sqref="A1:K2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>